<commit_message>
Fixed distance matrix normalization
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,14 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="clusterA" sheetId="1" r:id="rId1"/>
+    <sheet name="clusterB" sheetId="2" r:id="rId2"/>
+    <sheet name="rotationA" sheetId="3" r:id="rId3"/>
+    <sheet name="rotationB" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -332,17 +338,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -355,10 +361,170 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -368,17 +534,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -394,20 +560,316 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
         <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>6</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -418,7 +880,7 @@
         <v>3</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -426,31 +888,31 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new data examples
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,20 +9,22 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="clusterA" sheetId="1" r:id="rId1"/>
     <sheet name="clusterB" sheetId="2" r:id="rId2"/>
-    <sheet name="rotationA" sheetId="3" r:id="rId3"/>
-    <sheet name="rotationB" sheetId="4" r:id="rId4"/>
+    <sheet name="clusterA-v2" sheetId="5" r:id="rId3"/>
+    <sheet name="clusterB-v2" sheetId="6" r:id="rId4"/>
+    <sheet name="rotationB" sheetId="4" r:id="rId5"/>
+    <sheet name="rotationA" sheetId="3" r:id="rId6"/>
+    <sheet name="commA" sheetId="7" r:id="rId7"/>
+    <sheet name="commB" sheetId="8" r:id="rId8"/>
+    <sheet name="commA-v2" sheetId="9" r:id="rId9"/>
+    <sheet name="commB-v2" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -340,8 +342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,6 +527,162 @@
       </c>
       <c r="B23">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -725,10 +883,10 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B24">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -737,6 +895,310 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>7</v>
+      </c>
+      <c r="B14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>11</v>
+      </c>
+      <c r="B17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -756,71 +1218,71 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -828,7 +1290,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
@@ -848,71 +1310,491 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>12</v>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>7</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more data examples
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -539,14 +539,14 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -575,10 +575,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -586,12 +586,12 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -599,26 +599,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -663,26 +663,26 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B18">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1659,14 +1659,14 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B1">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1695,10 +1695,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1706,12 +1706,12 @@
         <v>2</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>4</v>
@@ -1719,26 +1719,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1783,18 +1783,18 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B16">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>